<commit_message>
Nov 4 Team Meeting Attendance
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week11.xlsx
+++ b/Admin/Gaby/TimeSheet_Week11.xlsx
@@ -361,15 +361,14 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,13 +502,15 @@
       <c r="D8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="10"/>
       <c r="I8" s="12" t="n">
         <f aca="false">SUM(B8:H8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="8"/>
     </row>
@@ -558,13 +559,15 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="10"/>
       <c r="I11" s="12" t="n">
         <f aca="false">SUM(B11:H11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="8"/>
     </row>
@@ -594,13 +597,15 @@
         <v>1</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="11"/>
       <c r="H13" s="10"/>
       <c r="I13" s="12" t="n">
         <f aca="false">SUM(B13:H13)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -622,7 +627,7 @@
       </c>
       <c r="E14" s="12" t="n">
         <f aca="false">SUM(E6:E13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14" s="12" t="n">
         <f aca="false">SUM(F6:F13)</f>
@@ -638,7 +643,7 @@
       </c>
       <c r="I14" s="12" t="n">
         <f aca="false">SUM(I6:I13)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
attendance and time sheets
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week11.xlsx
+++ b/Admin/Gaby/TimeSheet_Week11.xlsx
@@ -361,10 +361,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -601,11 +601,15 @@
         <v>2</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="10" t="n">
+        <v>4</v>
+      </c>
       <c r="I13" s="12" t="n">
         <f aca="false">SUM(B13:H13)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -635,15 +639,15 @@
       </c>
       <c r="G14" s="12" t="n">
         <f aca="false">SUM(G6:G13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="12" t="n">
         <f aca="false">SUM(H6:H13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I14" s="12" t="n">
         <f aca="false">SUM(I6:I13)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>